<commit_message>
ajout de verbien :la version qui fonction bien
</commit_message>
<xml_diff>
--- a/doubleData.xlsx
+++ b/doubleData.xlsx
@@ -11,18 +11,19 @@
     <sheet name="VEMS" sheetId="2" r:id="rId2"/>
     <sheet name="CVF" sheetId="3" r:id="rId3"/>
     <sheet name="CRF-He" sheetId="4" r:id="rId4"/>
-    <sheet name="CPT" sheetId="5" r:id="rId5"/>
+    <sheet name="CPT-he" sheetId="5" r:id="rId5"/>
     <sheet name="DEMM" sheetId="6" r:id="rId6"/>
     <sheet name="DEM25" sheetId="7" r:id="rId7"/>
     <sheet name="TEF" sheetId="8" r:id="rId8"/>
     <sheet name="CRFpl" sheetId="9" r:id="rId9"/>
+    <sheet name="CPTpl" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="119">
   <si>
     <t>NOM</t>
   </si>
@@ -126,58 +127,73 @@
     <t>0.37</t>
   </si>
   <si>
-    <t>CPT/Pré</t>
-  </si>
-  <si>
-    <t>CPT/Zscore</t>
-  </si>
-  <si>
-    <t>CPT/POST BD</t>
+    <t>CPT-he/Pré</t>
+  </si>
+  <si>
+    <t>CPT-he/Zscore</t>
+  </si>
+  <si>
+    <t>CPT-he/POST BD</t>
+  </si>
+  <si>
+    <t>5.82</t>
+  </si>
+  <si>
+    <t>DEMM/Pré</t>
+  </si>
+  <si>
+    <t>DEMM/Zscore</t>
+  </si>
+  <si>
+    <t>DEMM/POST effort</t>
+  </si>
+  <si>
+    <t>3.27</t>
+  </si>
+  <si>
+    <t>-0.92</t>
+  </si>
+  <si>
+    <t>DEM25/Pré</t>
+  </si>
+  <si>
+    <t>DEM25/Zscore</t>
+  </si>
+  <si>
+    <t>DEM25/POST effort</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>-1.00</t>
+  </si>
+  <si>
+    <t>TEF/Pré</t>
+  </si>
+  <si>
+    <t>TEF/Zscore</t>
+  </si>
+  <si>
+    <t>TEF/POST effort</t>
+  </si>
+  <si>
+    <t>4.85</t>
+  </si>
+  <si>
+    <t>CPTpl/Pré</t>
+  </si>
+  <si>
+    <t>CPTpl/Zscore</t>
+  </si>
+  <si>
+    <t>CPTpl/POST BD</t>
   </si>
   <si>
     <t>6.43</t>
   </si>
   <si>
-    <t>DEMM/Pré</t>
-  </si>
-  <si>
-    <t>DEMM/Zscore</t>
-  </si>
-  <si>
-    <t>DEMM/POST effort</t>
-  </si>
-  <si>
-    <t>3.27</t>
-  </si>
-  <si>
-    <t>-0.92</t>
-  </si>
-  <si>
-    <t>DEM25/Pré</t>
-  </si>
-  <si>
-    <t>DEM25/Zscore</t>
-  </si>
-  <si>
-    <t>DEM25/POST effort</t>
-  </si>
-  <si>
-    <t>1.25</t>
-  </si>
-  <si>
-    <t>-1.00</t>
-  </si>
-  <si>
-    <t>TEF/Pré</t>
-  </si>
-  <si>
-    <t>TEF/Zscore</t>
-  </si>
-  <si>
-    <t>TEF/POST effort</t>
-  </si>
-  <si>
-    <t>4.85</t>
+    <t>5.87</t>
   </si>
   <si>
     <t>Identification:</t>
@@ -210,21 +226,21 @@
     <t>0.02</t>
   </si>
   <si>
+    <t>-0.63</t>
+  </si>
+  <si>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>-0.79</t>
+  </si>
+  <si>
+    <t>3.96</t>
+  </si>
+  <si>
     <t>6.39</t>
   </si>
   <si>
-    <t>-0.63</t>
-  </si>
-  <si>
-    <t>1.36</t>
-  </si>
-  <si>
-    <t>-0.79</t>
-  </si>
-  <si>
-    <t>3.96</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -276,28 +292,31 @@
     <t>-1.29</t>
   </si>
   <si>
+    <t>3.47</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>2.06</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>5.11</t>
+  </si>
+  <si>
+    <t>6.13</t>
+  </si>
+  <si>
     <t>3.46</t>
   </si>
   <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
-    <t>2.06</t>
-  </si>
-  <si>
-    <t>0.47</t>
-  </si>
-  <si>
-    <t>0.84</t>
-  </si>
-  <si>
-    <t>5.11</t>
-  </si>
-  <si>
-    <t>6.13</t>
+    <t>3.57</t>
   </si>
   <si>
     <t>Cargol</t>
@@ -781,83 +800,238 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
       </c>
       <c r="H3" t="s">
         <v>56</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
+        <v>97</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" t="s">
-        <v>99</v>
+        <v>102</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -951,113 +1125,113 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="M3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="M4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="N4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="N5" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1130,83 +1304,83 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1264,19 +1438,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -1284,39 +1458,39 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1326,7 +1500,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1380,11 +1554,11 @@
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>37</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1392,28 +1566,28 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>37</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1421,28 +1595,28 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>89</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1450,140 +1624,27 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
+        <v>102</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
         <v>0</v>
       </c>
     </row>
@@ -1657,83 +1718,83 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1806,83 +1867,83 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="I5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1952,74 +2013,74 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="I5" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2077,19 +2138,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2097,39 +2158,39 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>